<commit_message>
useful figures and summary scores
</commit_message>
<xml_diff>
--- a/question analysis.xlsx
+++ b/question analysis.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hiroshimauniv-my.sharepoint.com/personal/d201901_hiroshima-u_ac_jp/Documents/Doctoral Course 2020/Experiments/OOP_Maya/last experiment files/OOP-experiment-data-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{60F4B845-900B-45FA-9933-3F8294C0525D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92D81B41-DEFB-4F75-BF9C-5FB83A10D2A6}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="8_{60F4B845-900B-45FA-9933-3F8294C0525D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDE028D7-4F02-48CF-987E-EC0FF5A96707}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1305" windowWidth="29040" windowHeight="15720" xr2:uid="{DF46B937-C84B-475E-9132-1CA2D10F79F5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DF46B937-C84B-475E-9132-1CA2D10F79F5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="question category" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="71">
   <si>
     <t>q1</t>
   </si>
@@ -221,13 +221,40 @@
   </si>
   <si>
     <t>SUM</t>
+  </si>
+  <si>
+    <t>related to two classes, encapsulation -access- and inheritance</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>Bloom</t>
+  </si>
+  <si>
+    <t>Remember</t>
+  </si>
+  <si>
+    <t>Understand</t>
+  </si>
+  <si>
+    <t>Apply</t>
+  </si>
+  <si>
+    <t>Analyze</t>
+  </si>
+  <si>
+    <t>Evaluate</t>
+  </si>
+  <si>
+    <t>Create</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,8 +268,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,20 +299,23 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -277,16 +328,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -315,19 +373,19 @@
     <tableColumn id="3" xr3:uid="{31BE6917-8DD4-41DD-BCE7-3FB7BC8FAFF1}" name="Q2"/>
     <tableColumn id="4" xr3:uid="{7A45B43A-7A7B-4F51-9A63-80270DC5D26B}" name="Q3"/>
     <tableColumn id="5" xr3:uid="{E6E37387-0F49-40DD-9C0D-0425B76A148C}" name="Q4"/>
-    <tableColumn id="6" xr3:uid="{169A3653-D1F1-431F-928B-1A4B258419DC}" name="Q5"/>
+    <tableColumn id="6" xr3:uid="{169A3653-D1F1-431F-928B-1A4B258419DC}" name="Q5" dataCellStyle="Good"/>
     <tableColumn id="7" xr3:uid="{A05042FA-8D37-462F-889F-35AB781D47C6}" name="Q6"/>
     <tableColumn id="8" xr3:uid="{C98456F5-B715-443B-96A7-43CB64FC0A83}" name="Q7"/>
     <tableColumn id="9" xr3:uid="{CFEA0940-CA85-4AA1-BE33-F3C1F65337E2}" name="Q8"/>
     <tableColumn id="10" xr3:uid="{AAA8302E-0C33-4516-9B28-67F363B20434}" name="Q9"/>
     <tableColumn id="11" xr3:uid="{563162CE-8C9C-46A8-9B2E-56665B588067}" name="Q10"/>
-    <tableColumn id="12" xr3:uid="{FF94D589-8F3A-4022-BF9A-E33C4A16A43D}" name="Q11"/>
-    <tableColumn id="13" xr3:uid="{A4BA1B33-442C-4235-AFF6-3F2302192F15}" name="Q12"/>
+    <tableColumn id="12" xr3:uid="{FF94D589-8F3A-4022-BF9A-E33C4A16A43D}" name="Q11" dataCellStyle="Bad"/>
+    <tableColumn id="13" xr3:uid="{A4BA1B33-442C-4235-AFF6-3F2302192F15}" name="Q12" dataCellStyle="Good"/>
     <tableColumn id="14" xr3:uid="{52BEFB84-2BE2-4A54-99B8-3C4AA7A06B66}" name="Q13"/>
-    <tableColumn id="15" xr3:uid="{15464CB4-3F6B-444C-8896-9A2D8883CE60}" name="Q14"/>
+    <tableColumn id="15" xr3:uid="{15464CB4-3F6B-444C-8896-9A2D8883CE60}" name="Q14" dataCellStyle="Bad"/>
     <tableColumn id="16" xr3:uid="{43E849F9-82D3-4533-9B40-7F1F60D3BA72}" name="Q15"/>
-    <tableColumn id="17" xr3:uid="{3F9B4245-E813-463D-AECF-158A5B2F48AC}" name="Q16"/>
-    <tableColumn id="18" xr3:uid="{4F06E860-86A6-4463-8396-DAE788A3A413}" name="Q17"/>
+    <tableColumn id="17" xr3:uid="{3F9B4245-E813-463D-AECF-158A5B2F48AC}" name="Q16" dataCellStyle="Bad"/>
+    <tableColumn id="18" xr3:uid="{4F06E860-86A6-4463-8396-DAE788A3A413}" name="Q17" dataCellStyle="Good"/>
     <tableColumn id="19" xr3:uid="{26B41AA4-856E-4771-9189-3DC2A44BA98F}" name="Q18"/>
     <tableColumn id="20" xr3:uid="{9133FFC9-A8B3-4841-BDE8-582EBD8EE391}" name="Q19"/>
     <tableColumn id="21" xr3:uid="{F8A282F0-3901-463D-9D65-C1D10516B26D}" name="Q20"/>
@@ -639,215 +697,294 @@
   <dimension ref="A1:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="21" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4.8872180000000001E-2</v>
       </c>
       <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="U2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>0.22222222</v>
       </c>
       <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="U3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
+        <v>9.5238100000000006E-2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="U4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.15476190000000001</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="U5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.50724638</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="U6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
       <c r="B7">
-        <v>1</v>
+        <v>5.2631579999999997E-2</v>
       </c>
       <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="U7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>0.28571428999999998</v>
       </c>
       <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-1</v>
+        <v>-4.0404040000000002E-2</v>
       </c>
       <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>0.45714285999999998</v>
       </c>
       <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>0.17521368000000001</v>
       </c>
       <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-4</v>
+        <v>-0.14822134000000001</v>
       </c>
       <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>9</v>
+        <v>0.5</v>
       </c>
       <c r="C13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>0.19473683999999999</v>
       </c>
       <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-2</v>
+        <v>-0.33333332999999998</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>4.923077E-2</v>
       </c>
       <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>-3</v>
+        <v>-0.17777778</v>
       </c>
       <c r="C17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>8</v>
+        <v>0.57142857000000002</v>
       </c>
       <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>5.2631579999999997E-2</v>
       </c>
       <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
         <v>36</v>
       </c>
     </row>
@@ -856,27 +993,27 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>0.1995614</v>
       </c>
       <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>-6.25E-2</v>
       </c>
       <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="E22">
-        <f>3/(41-38)</f>
-        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -948,133 +1085,133 @@
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3">
-        <v>1</v>
-      </c>
-      <c r="E26" s="3">
-        <v>1</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3">
-        <v>1</v>
-      </c>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3">
+      <c r="M26" s="2"/>
+      <c r="N26" s="1">
         <v>1</v>
       </c>
       <c r="O26" s="3">
         <v>1</v>
       </c>
-      <c r="P26" s="3"/>
+      <c r="P26" s="1"/>
       <c r="Q26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="S26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
+      <c r="R26" s="2"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
       <c r="V26">
         <f>SUM(Table1[[#This Row],[Q1]:[Q20]])</f>
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3">
-        <v>1</v>
-      </c>
-      <c r="I27" s="3">
-        <v>1</v>
-      </c>
-      <c r="J27" s="3">
-        <v>1</v>
-      </c>
-      <c r="K27" s="3">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1">
         <v>1</v>
       </c>
       <c r="L27" s="3">
         <v>1</v>
       </c>
-      <c r="M27" s="3">
-        <v>1</v>
-      </c>
-      <c r="N27" s="3"/>
+      <c r="M27" s="2">
+        <v>1</v>
+      </c>
+      <c r="N27" s="1"/>
       <c r="O27" s="3"/>
-      <c r="P27" s="3">
+      <c r="P27" s="1">
         <v>1</v>
       </c>
       <c r="Q27" s="3">
         <v>1</v>
       </c>
-      <c r="R27" s="3">
-        <v>1</v>
-      </c>
-      <c r="S27" s="3">
-        <v>1</v>
-      </c>
-      <c r="T27" s="3">
-        <v>1</v>
-      </c>
-      <c r="U27" s="3"/>
+      <c r="R27" s="2">
+        <v>1</v>
+      </c>
+      <c r="S27" s="1">
+        <v>1</v>
+      </c>
+      <c r="T27" s="1">
+        <v>1</v>
+      </c>
+      <c r="U27" s="1"/>
       <c r="V27">
         <f>SUM(Table1[[#This Row],[Q1]:[Q20]])</f>
         <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="3">
-        <v>1</v>
-      </c>
-      <c r="C28" s="3">
-        <v>1</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3">
-        <v>1</v>
-      </c>
-      <c r="G28" s="3">
-        <v>1</v>
-      </c>
-      <c r="H28" s="3">
-        <v>1</v>
-      </c>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
       <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3">
+      <c r="M28" s="2"/>
+      <c r="N28" s="1">
         <v>1</v>
       </c>
       <c r="O28" s="3">
         <v>1</v>
       </c>
-      <c r="P28" s="3"/>
+      <c r="P28" s="1"/>
       <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3"/>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3">
+      <c r="R28" s="2"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1">
         <v>1</v>
       </c>
       <c r="V28">
@@ -1096,6 +1233,11 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C21" xr:uid="{E9376FB2-3F1A-45DF-A7C8-7AA323D04E93}">
+      <formula1>$U$2:$U$7</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>